<commit_message>
Modified schematic and board files slightly
</commit_message>
<xml_diff>
--- a/hdw/AC_Power_Meter/AC_Power_Meter_bom.xlsx
+++ b/hdw/AC_Power_Meter/AC_Power_Meter_bom.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\AC_Power_Meter\hdw\AC_Power_Meter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{77885F7E-D370-43A8-AAE4-676DB3D44158}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC41A2E4-047B-4EC1-ABE2-47C8BDB68A8E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16000" windowHeight="6340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AC_Power_Meter_bom_A" sheetId="1" r:id="rId1"/>
@@ -703,11 +703,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -838,6 +838,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1184,7 +1191,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1199,6 +1206,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1553,22 +1563,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.36328125" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" style="5"/>
     <col min="8" max="8" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1603,7 +1613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="203" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1630,8 +1640,8 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1657,8 +1667,8 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1684,8 +1694,8 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1711,8 +1721,8 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1738,8 +1748,8 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1765,8 +1775,8 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1792,8 +1802,8 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1819,8 +1829,8 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1846,8 +1856,8 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1873,8 +1883,8 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1900,8 +1910,8 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1927,8 +1937,8 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1948,8 +1958,8 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1969,8 +1979,8 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1992,8 +2002,8 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2015,8 +2025,8 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2038,8 +2048,8 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2059,8 +2069,8 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2080,7 +2090,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -2099,7 +2109,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>78</v>
       </c>
@@ -2118,7 +2128,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>80</v>
       </c>
@@ -2139,7 +2149,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>83</v>
       </c>
@@ -2160,7 +2170,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>85</v>
       </c>
@@ -2181,7 +2191,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>87</v>
       </c>
@@ -2202,7 +2212,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>89</v>
       </c>
@@ -2223,7 +2233,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>91</v>
       </c>
@@ -2244,7 +2254,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>93</v>
       </c>
@@ -2265,7 +2275,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>96</v>
       </c>
@@ -2284,7 +2294,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>99</v>
       </c>
@@ -2305,8 +2315,8 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2332,8 +2342,8 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2353,7 +2363,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>109</v>
       </c>
@@ -2374,7 +2384,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>112</v>
       </c>
@@ -2395,7 +2405,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>116</v>
       </c>
@@ -2414,7 +2424,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>117</v>
       </c>
@@ -2433,7 +2443,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>120</v>
       </c>
@@ -2454,7 +2464,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>122</v>
       </c>
@@ -2475,7 +2485,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>126</v>
       </c>
@@ -2496,7 +2506,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>129</v>
       </c>
@@ -2515,7 +2525,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>131</v>
       </c>
@@ -2536,8 +2546,8 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
         <v>133</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2557,8 +2567,8 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
         <v>136</v>
       </c>
       <c r="B44" s="1">
@@ -2584,8 +2594,8 @@
       </c>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
         <v>139</v>
       </c>
       <c r="B45" s="1">
@@ -2611,8 +2621,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
         <v>141</v>
       </c>
       <c r="B46" s="1">
@@ -2638,8 +2648,8 @@
       </c>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2665,8 +2675,8 @@
       </c>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2692,8 +2702,8 @@
       </c>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:11" ht="232" x14ac:dyDescent="0.35">
+      <c r="A49" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2719,8 +2729,8 @@
       </c>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A50" s="6" t="s">
         <v>152</v>
       </c>
       <c r="B50" s="1">
@@ -2746,8 +2756,8 @@
       </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A51" s="6" t="s">
         <v>155</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2773,8 +2783,8 @@
       </c>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A52" s="6" t="s">
         <v>158</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2800,8 +2810,8 @@
       </c>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53" s="6" t="s">
         <v>161</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2827,8 +2837,8 @@
       </c>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A54" s="6" t="s">
         <v>163</v>
       </c>
       <c r="B54" s="1">
@@ -2854,8 +2864,8 @@
       </c>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A55" s="6" t="s">
         <v>165</v>
       </c>
       <c r="B55" s="1">
@@ -2881,8 +2891,8 @@
       </c>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A56" s="6" t="s">
         <v>167</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2908,8 +2918,8 @@
       </c>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A57" s="6" t="s">
         <v>170</v>
       </c>
       <c r="B57" s="1">
@@ -2935,8 +2945,8 @@
       </c>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A58" s="6" t="s">
         <v>172</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2962,8 +2972,8 @@
       </c>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A59" s="6" t="s">
         <v>175</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -2989,8 +2999,8 @@
       </c>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A60" s="6" t="s">
         <v>178</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -3016,7 +3026,7 @@
       </c>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>181</v>
       </c>
@@ -3035,8 +3045,8 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A62" s="6" t="s">
         <v>183</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -3056,8 +3066,8 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A63" s="6" t="s">
         <v>186</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -3077,7 +3087,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>189</v>
       </c>
@@ -3098,8 +3108,8 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A65" s="6" t="s">
         <v>193</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -3119,8 +3129,8 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A66" s="6" t="s">
         <v>196</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -3140,8 +3150,8 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A67" s="6" t="s">
         <v>199</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -3161,8 +3171,8 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="6" t="s">
         <v>202</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -3182,8 +3192,8 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69" s="6" t="s">
         <v>205</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -3203,8 +3213,8 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A70" s="6" t="s">
         <v>208</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -3224,8 +3234,8 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="6" t="s">
         <v>210</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -3245,7 +3255,7 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>214</v>
       </c>
@@ -3264,8 +3274,8 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A73" s="6" t="s">
         <v>216</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -3285,8 +3295,8 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="6" t="s">
         <v>218</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -3306,8 +3316,8 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A75" s="6" t="s">
         <v>221</v>
       </c>
       <c r="B75" s="1" t="s">

</xml_diff>

<commit_message>
Fixed ISNS DC offset issue
</commit_message>
<xml_diff>
--- a/hdw/AC_Power_Meter/AC_Power_Meter_bom.xlsx
+++ b/hdw/AC_Power_Meter/AC_Power_Meter_bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\AC_Power_Meter\hdw\AC_Power_Meter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC41A2E4-047B-4EC1-ABE2-47C8BDB68A8E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A135D2-1337-4725-98DC-B36C0427D9F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16000" windowHeight="6340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -844,7 +844,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1566,20 +1565,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" style="6" customWidth="1"/>
     <col min="4" max="4" width="23.36328125" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" style="5"/>
     <col min="8" max="8" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1614,7 +1611,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="203" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2091,7 +2088,7 @@
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="6" t="s">
         <v>77</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2110,7 +2107,7 @@
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="6" t="s">
         <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2129,7 +2126,7 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="6" t="s">
         <v>80</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2150,7 +2147,7 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="6" t="s">
         <v>83</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2171,7 +2168,7 @@
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2192,7 +2189,7 @@
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="6" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2213,7 +2210,7 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2234,7 +2231,7 @@
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="6" t="s">
         <v>91</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2255,7 +2252,7 @@
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="6" t="s">
         <v>93</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2276,7 +2273,7 @@
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="6" t="s">
         <v>96</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2295,7 +2292,7 @@
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2364,7 +2361,7 @@
       <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2385,7 +2382,7 @@
       <c r="K34" s="1"/>
     </row>
     <row r="35" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2406,7 +2403,7 @@
       <c r="K35" s="1"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="6" t="s">
         <v>116</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2425,7 +2422,7 @@
       <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="6" t="s">
         <v>117</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2444,7 +2441,7 @@
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="6" t="s">
         <v>120</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2465,7 +2462,7 @@
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="6" t="s">
         <v>122</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2486,7 +2483,7 @@
       <c r="K39" s="1"/>
     </row>
     <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="6" t="s">
         <v>126</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2507,7 +2504,7 @@
       <c r="K40" s="1"/>
     </row>
     <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="6" t="s">
         <v>129</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2526,7 +2523,7 @@
       <c r="K41" s="1"/>
     </row>
     <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="6" t="s">
         <v>131</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -3027,7 +3024,7 @@
       <c r="K60" s="1"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="6" t="s">
         <v>181</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -3088,7 +3085,7 @@
       <c r="K63" s="1"/>
     </row>
     <row r="64" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -3256,7 +3253,7 @@
       <c r="K71" s="1"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="6" t="s">
         <v>214</v>
       </c>
       <c r="B72" s="1" t="s">

</xml_diff>